<commit_message>
Feature Addition: Scheduled mail for leaderwise report
</commit_message>
<xml_diff>
--- a/main/res/leader_report/Leaderwise_Report_05_29_2020.xlsx
+++ b/main/res/leader_report/Leaderwise_Report_05_29_2020.xlsx
@@ -14,18 +14,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+  <si>
+    <t>LEADER: 9407829662</t>
+  </si>
+  <si>
+    <t>PHONE</t>
+  </si>
+  <si>
+    <t>Number of Translations</t>
+  </si>
+  <si>
+    <t>9407829662</t>
+  </si>
+  <si>
+    <t>7747091774</t>
+  </si>
+  <si>
+    <t>7067496684</t>
+  </si>
+  <si>
+    <t>7796455948</t>
+  </si>
+  <si>
+    <t>9098996282</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>LEADER: 9421796504</t>
+  </si>
+  <si>
+    <t>9421796504</t>
+  </si>
+  <si>
+    <t>9405812428</t>
+  </si>
+  <si>
+    <t>9422001930</t>
+  </si>
+  <si>
+    <t>9403471299</t>
+  </si>
+  <si>
+    <t>9403624706</t>
+  </si>
+  <si>
+    <t>LEADER: 9131479289</t>
+  </si>
+  <si>
+    <t>9131479289</t>
+  </si>
+  <si>
+    <t>LEADER: 8763134297</t>
+  </si>
+  <si>
+    <t>8763134297</t>
+  </si>
+  <si>
+    <t>9439191433</t>
+  </si>
+  <si>
+    <t>9777519828</t>
+  </si>
+  <si>
+    <t>9770199903</t>
+  </si>
+  <si>
+    <t>8658839633</t>
+  </si>
+  <si>
+    <t>9438859084</t>
+  </si>
+  <si>
+    <t>8895113188</t>
+  </si>
+  <si>
+    <t>9438782004</t>
+  </si>
+  <si>
+    <t>LEADER: 7083879756</t>
+  </si>
+  <si>
+    <t>7083879756</t>
+  </si>
+  <si>
+    <t>9922475025</t>
+  </si>
+  <si>
+    <t>8888412205</t>
+  </si>
+  <si>
+    <t>8698808566</t>
+  </si>
+  <si>
+    <t>9850082353</t>
+  </si>
+  <si>
+    <t>7588101154</t>
+  </si>
+  <si>
+    <t>9405726232</t>
+  </si>
+  <si>
+    <t>7083408705</t>
+  </si>
+  <si>
+    <t>9527354040</t>
+  </si>
+  <si>
+    <t>7066800205</t>
+  </si>
+  <si>
+    <t>LEADER: 7287917104</t>
+  </si>
+  <si>
+    <t>7287917104</t>
+  </si>
+  <si>
+    <t>7032595636</t>
+  </si>
+  <si>
+    <t>9491344726</t>
+  </si>
+  <si>
+    <t>9603999439</t>
+  </si>
+  <si>
+    <t>LEADER: 7000432750</t>
+  </si>
+  <si>
+    <t>7000432750</t>
+  </si>
+  <si>
+    <t>6263236094</t>
+  </si>
+  <si>
+    <t>9340891699</t>
+  </si>
+  <si>
+    <t>9691246080</t>
+  </si>
+  <si>
+    <t>8770851549</t>
+  </si>
+  <si>
+    <t>7049347202</t>
+  </si>
+  <si>
+    <t>9993948351</t>
+  </si>
+  <si>
+    <t>8839225164</t>
+  </si>
+  <si>
+    <t>9009512687</t>
+  </si>
+  <si>
+    <t>9407298180</t>
+  </si>
+  <si>
+    <t>7000301143</t>
+  </si>
+  <si>
+    <t>9303215150</t>
+  </si>
   <si>
     <t>LEADER: 6267034661</t>
   </si>
   <si>
-    <t>PHONE</t>
-  </si>
-  <si>
-    <t>Number of Translations</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>6267034661</t>
   </si>
 </sst>
 </file>
@@ -390,7 +549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,15 +571,480 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
         <v>3</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>2759</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A60:B60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>